<commit_message>
Updated stats for Apr 8
</commit_message>
<xml_diff>
--- a/Covid19 US Cases Tracking (Excel).xlsx
+++ b/Covid19 US Cases Tracking (Excel).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Brian/Dropbox/Programming/Projects/DS Projects/CoronaVirus/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35AFB2A1-3D11-3042-8CB9-C57A9F7F6728}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE0BCB57-5E4F-5E4E-959D-CE9F18B0A8E5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="26880" yWindow="-360" windowWidth="38400" windowHeight="21140" xr2:uid="{2DCD77F1-C1DF-40E4-8CFE-958F60BFDE9D}"/>
   </bookViews>
@@ -607,7 +607,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I41" sqref="I41"/>
+      <selection pane="bottomLeft" activeCell="I42" sqref="I42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" outlineLevelCol="2" x14ac:dyDescent="0.2"/>
@@ -2647,29 +2647,28 @@
         <f t="shared" si="29"/>
         <v>43929</v>
       </c>
-      <c r="I42" s="15">
-        <f t="shared" ref="I42:I48" si="34">I41*(1+AVERAGE(M39:M41))</f>
-        <v>435326.70134513138</v>
+      <c r="I42" s="14">
+        <v>434927</v>
       </c>
       <c r="J42" s="21">
         <f t="shared" si="30"/>
-        <v>-3363715.2986548687</v>
+        <v>-3364115</v>
       </c>
       <c r="K42" s="22">
         <f t="shared" si="18"/>
-        <v>1330.4605786831644</v>
+        <v>1329.2389975550122</v>
       </c>
       <c r="L42" s="21">
         <f t="shared" si="31"/>
-        <v>34991.701345131383</v>
+        <v>34592</v>
       </c>
       <c r="M42" s="23">
         <f t="shared" si="32"/>
-        <v>8.7406050795287404E-2</v>
+        <v>8.6407633606854259E-2</v>
       </c>
       <c r="N42" s="23">
         <f t="shared" si="33"/>
-        <v>-0.24439672237690313</v>
+        <v>-0.24539513956533626</v>
       </c>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.2">
@@ -2701,28 +2700,28 @@
         <v>43930</v>
       </c>
       <c r="I43" s="15">
-        <f t="shared" si="34"/>
-        <v>474261.68432089838</v>
+        <f t="shared" ref="I42:I48" si="34">I42*(1+AVERAGE(M40:M42))</f>
+        <v>473681.48807500117</v>
       </c>
       <c r="J43" s="21">
         <f t="shared" si="30"/>
-        <v>-4585313.3156791013</v>
+        <v>-4585893.5119249988</v>
       </c>
       <c r="K43" s="22">
         <f t="shared" si="18"/>
-        <v>1449.4550254306184</v>
+        <v>1447.6818095201747</v>
       </c>
       <c r="L43" s="21">
         <f t="shared" si="31"/>
-        <v>38934.982975766994</v>
+        <v>38754.488075001165</v>
       </c>
       <c r="M43" s="23">
         <f t="shared" si="32"/>
-        <v>8.9438536288861697E-2</v>
+        <v>8.9105730559383908E-2</v>
       </c>
       <c r="N43" s="23">
         <f t="shared" si="33"/>
-        <v>-0.24236423688332884</v>
+        <v>-0.24269704261280661</v>
       </c>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.2">
@@ -2755,27 +2754,27 @@
       </c>
       <c r="I44" s="15">
         <f t="shared" si="34"/>
-        <v>516575.90631735633</v>
+        <v>515733.75235084363</v>
       </c>
       <c r="J44" s="21">
         <f t="shared" si="30"/>
-        <v>-6221780.093682644</v>
+        <v>-6222622.2476491565</v>
       </c>
       <c r="K44" s="22">
         <f t="shared" si="18"/>
-        <v>1578.7772197963213</v>
+        <v>1576.2033996052678</v>
       </c>
       <c r="L44" s="21">
         <f t="shared" si="31"/>
-        <v>42314.221996457956</v>
+        <v>42052.264275842463</v>
       </c>
       <c r="M44" s="23">
         <f t="shared" si="32"/>
-        <v>8.9221253572377993E-2</v>
+        <v>8.8777512599740954E-2</v>
       </c>
       <c r="N44" s="23">
         <f t="shared" si="33"/>
-        <v>-0.24258151959981256</v>
+        <v>-0.24302526057244958</v>
       </c>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.2">
@@ -2808,27 +2807,27 @@
       </c>
       <c r="I45" s="15">
         <f t="shared" si="34"/>
-        <v>562390.30724310118</v>
+        <v>561168.32754638128</v>
       </c>
       <c r="J45" s="21">
         <f t="shared" si="30"/>
-        <v>-8411770.6927568987</v>
+        <v>-8412992.6724536195</v>
       </c>
       <c r="K45" s="22">
         <f t="shared" si="18"/>
-        <v>1718.7967825278154</v>
+        <v>1715.062125752999</v>
       </c>
       <c r="L45" s="21">
         <f t="shared" si="31"/>
-        <v>45814.400925744849</v>
+        <v>45434.575195537647</v>
       </c>
       <c r="M45" s="23">
         <f t="shared" si="32"/>
-        <v>8.8688613552175541E-2</v>
+        <v>8.8096958921993124E-2</v>
       </c>
       <c r="N45" s="23">
         <f t="shared" si="33"/>
-        <v>-0.24311415962001498</v>
+        <v>-0.24370581425019741</v>
       </c>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.2">
@@ -2861,27 +2860,27 @@
       </c>
       <c r="I46" s="15">
         <f t="shared" si="34"/>
-        <v>612508.35748864221</v>
+        <v>610921.54926715104</v>
       </c>
       <c r="J46" s="21">
         <f t="shared" si="30"/>
-        <v>-11339304.642511358</v>
+        <v>-11340891.45073285</v>
       </c>
       <c r="K46" s="22">
         <f t="shared" si="18"/>
-        <v>1871.969307728124</v>
+        <v>1867.1196493494838</v>
       </c>
       <c r="L46" s="21">
         <f t="shared" si="31"/>
-        <v>50118.050245541031</v>
+        <v>49753.221720769769</v>
       </c>
       <c r="M46" s="23">
         <f t="shared" si="32"/>
-        <v>8.9116134471138378E-2</v>
+        <v>8.8660067360372546E-2</v>
       </c>
       <c r="N46" s="23">
         <f t="shared" si="33"/>
-        <v>-0.24268663870105217</v>
+        <v>-0.24314270581181799</v>
       </c>
       <c r="O46" t="s">
         <v>19</v>
@@ -2917,27 +2916,27 @@
       </c>
       <c r="I47" s="15">
         <f t="shared" si="34"/>
-        <v>667026.91003668774</v>
+        <v>664995.13989308267</v>
       </c>
       <c r="J47" s="21">
         <f t="shared" si="30"/>
-        <v>-15250431.089963313</v>
+        <v>-15252462.860106917</v>
       </c>
       <c r="K47" s="22">
         <f t="shared" si="18"/>
-        <v>2038.5908008456227</v>
+        <v>2032.381234392062</v>
       </c>
       <c r="L47" s="21">
         <f t="shared" si="31"/>
-        <v>54518.552548045525</v>
+        <v>54073.590625931625</v>
       </c>
       <c r="M47" s="23">
         <f t="shared" si="32"/>
-        <v>8.9008667198563846E-2</v>
+        <v>8.851151296070206E-2</v>
       </c>
       <c r="N47" s="23">
         <f t="shared" si="33"/>
-        <v>-0.24279410597362669</v>
+        <v>-0.24329126021148847</v>
       </c>
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.2">
@@ -2970,27 +2969,27 @@
       </c>
       <c r="I48" s="15">
         <f t="shared" si="34"/>
-        <v>726350.81934061612</v>
+        <v>723795.90301414183</v>
       </c>
       <c r="J48" s="21">
         <f t="shared" si="30"/>
-        <v>-20472564.180659384</v>
+        <v>-20475119.096985858</v>
       </c>
       <c r="K48" s="22">
         <f t="shared" si="18"/>
-        <v>2219.8985921167973</v>
+        <v>2212.0901681361302</v>
       </c>
       <c r="L48" s="21">
         <f t="shared" si="31"/>
-        <v>59323.909303928376</v>
+        <v>58800.763121059164</v>
       </c>
       <c r="M48" s="23">
         <f t="shared" si="32"/>
-        <v>8.8937805073959389E-2</v>
+        <v>8.8422846414355896E-2</v>
       </c>
       <c r="N48" s="23">
         <f t="shared" si="33"/>
-        <v>-0.24286496809823116</v>
+        <v>-0.24337992675783465</v>
       </c>
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.2">
@@ -3023,27 +3022,27 @@
       </c>
       <c r="I49" s="15">
         <f t="shared" ref="I49" si="36">I48*(1+AVERAGE(M46:M48))</f>
-        <v>791011.20041511592</v>
+        <v>787874.62232563982</v>
       </c>
       <c r="J49" s="21">
         <f t="shared" ref="J49" si="37">IF(I49&lt;=0,0, I49-B49)</f>
-        <v>-27441762.799584884</v>
+        <v>-27444899.37767436</v>
       </c>
       <c r="K49" s="22">
         <f t="shared" si="18"/>
-        <v>2417.5158936892299</v>
+        <v>2407.9297748338627</v>
       </c>
       <c r="L49" s="21">
         <f t="shared" ref="L49" si="38">IF(I49&lt;=0,0, I49-I48)</f>
-        <v>64660.381074499805</v>
+        <v>64078.719311497989</v>
       </c>
       <c r="M49" s="23">
         <f t="shared" ref="M49" si="39">IF(I49&lt;=0,0, L49/I48)</f>
-        <v>8.9020868914553894E-2</v>
+        <v>8.8531475578476695E-2</v>
       </c>
       <c r="N49" s="23">
         <f t="shared" ref="N49" si="40">IF(I49&lt;=0,0,M49-E49)</f>
-        <v>-0.24278190425763663</v>
+        <v>-0.24327129759371385</v>
       </c>
     </row>
     <row r="53" spans="1:14" x14ac:dyDescent="0.2">

</xml_diff>